<commit_message>
fix sheet 2022.07.23, 2022.07.25
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/ThongDiep/BANG_KE_THONG_DIEP.xlsx
+++ b/API/wwwroot/docs/ThongDiep/BANG_KE_THONG_DIEP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\ThongDiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pmbk\bills\bill-back-end\API\wwwroot\docs\ThongDiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="990" yWindow="990" windowWidth="15000" windowHeight="9990"/>
+    <workbookView xWindow="996" yWindow="996" windowWidth="15000" windowHeight="9996"/>
   </bookViews>
   <sheets>
     <sheet name="HOADON-BACHKHOA" sheetId="1" r:id="rId1"/>
@@ -519,21 +519,20 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="18" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="3"/>
+    <col min="3" max="3" width="24.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="51.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -546,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -561,7 +560,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -590,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -601,7 +600,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>2</v>

</xml_diff>